<commit_message>
updated test matric per richard
</commit_message>
<xml_diff>
--- a/docs/UC-TestMatrix.xlsx
+++ b/docs/UC-TestMatrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="127">
   <si>
     <t>Unified Client Agent Project - Test Matrix</t>
   </si>
@@ -168,15 +168,6 @@
     <t>Linux - Ubuntu                                     Join Domain</t>
   </si>
   <si>
-    <t>Linux - Linux variation:  xxxxxx     Join Domain</t>
-  </si>
-  <si>
-    <t>Linux - Linux variation:  xxxxxx     UnJoin Domain</t>
-  </si>
-  <si>
-    <t>Linux - Linux variation:  xxxxxx     Reboot</t>
-  </si>
-  <si>
     <t>7a</t>
   </si>
   <si>
@@ -228,24 +219,12 @@
     <t>5e</t>
   </si>
   <si>
-    <t>6d</t>
-  </si>
-  <si>
-    <t>6e</t>
-  </si>
-  <si>
     <t>Linux - Ubuntu                                    Asset Update</t>
   </si>
   <si>
-    <t>Linux - Linux variation:  xxxxxx     Asset Update</t>
-  </si>
-  <si>
     <t>Linux - Ubuntu                                    Auto EIL Update</t>
   </si>
   <si>
-    <t>Linux - Linux variation:  xxxxxx     Auto EIL Update</t>
-  </si>
-  <si>
     <t>Resolution Date</t>
   </si>
   <si>
@@ -255,12 +234,6 @@
     <t>7c</t>
   </si>
   <si>
-    <t>7e</t>
-  </si>
-  <si>
-    <t>7d</t>
-  </si>
-  <si>
     <t>3d</t>
   </si>
   <si>
@@ -277,6 +250,153 @@
   </si>
   <si>
     <t>Linux Client - Lab Physical              EIL Deployment</t>
+  </si>
+  <si>
+    <t>OS version</t>
+  </si>
+  <si>
+    <t>Windows 7 Ent 64</t>
+  </si>
+  <si>
+    <t>XP sp3 32 bit</t>
+  </si>
+  <si>
+    <t>NT Svr 2003 SP1 32</t>
+  </si>
+  <si>
+    <t>Linux: Ubuntu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supported Linux platforms (RHEL, CentOS, Ubuntu, Slackware, Slax, SuSE, XenClient/XenServer etc.) </t>
+  </si>
+  <si>
+    <t>Linux:  RHEL</t>
+  </si>
+  <si>
+    <t>Linux:  CentOS</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  RHEL        Auto EIL Update</t>
+  </si>
+  <si>
+    <t>17a</t>
+  </si>
+  <si>
+    <t>17b</t>
+  </si>
+  <si>
+    <t>17c</t>
+  </si>
+  <si>
+    <t>17d</t>
+  </si>
+  <si>
+    <t>17e</t>
+  </si>
+  <si>
+    <t>Linux:  Slackware</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  Slackware     Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  Slackware     Asset Update</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  Slackware     Auto EIL Update</t>
+  </si>
+  <si>
+    <t>8a</t>
+  </si>
+  <si>
+    <t>8b</t>
+  </si>
+  <si>
+    <t>8c</t>
+  </si>
+  <si>
+    <t>Linux:  Slax</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  RHEL        Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  RHEL        Asset Update</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  CentOS   Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  CentOS   Asset Update</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  CentOS   Auto EIL Update</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  Slax        Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  Slax        Asset Update</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>10b</t>
+  </si>
+  <si>
+    <t>11c</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  SuSE       Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:  SuSE        Asset Update</t>
+  </si>
+  <si>
+    <t>Linux:  SuSE</t>
+  </si>
+  <si>
+    <t>9b</t>
+  </si>
+  <si>
+    <t>9c</t>
+  </si>
+  <si>
+    <t>10a</t>
+  </si>
+  <si>
+    <t>10c</t>
+  </si>
+  <si>
+    <t>Linux:   XenClient/XenServer</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:   XenClient/XenServer  Reboot</t>
+  </si>
+  <si>
+    <t>Linux - Linux variation:   XenClient/XenServer  Asset Update</t>
+  </si>
+  <si>
+    <t>11a</t>
+  </si>
+  <si>
+    <t>11b</t>
+  </si>
+  <si>
+    <t>Unbuntudev3</t>
+  </si>
+  <si>
+    <t>Unbuntudev4</t>
+  </si>
+  <si>
+    <t>Unbuntudev5</t>
+  </si>
+  <si>
+    <t>Unbuntudev6</t>
+  </si>
+  <si>
+    <t>Unbuntudev7</t>
   </si>
 </sst>
 </file>
@@ -622,30 +742,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.28515625" customWidth="1"/>
-    <col min="2" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -653,34 +775,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -688,84 +813,87 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -773,84 +901,87 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -858,84 +989,87 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -943,84 +1077,87 @@
         <v>38</v>
       </c>
       <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
       <c r="E21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
       <c r="E23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
         <v>64</v>
       </c>
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>15</v>
       </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1028,251 +1165,507 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
       <c r="E27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>16</v>
       </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
       <c r="E28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="D29" t="s">
-        <v>17</v>
-      </c>
       <c r="E29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D31" t="s">
         <v>16</v>
       </c>
-      <c r="D30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" t="s">
+        <v>124</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" t="s">
+        <v>126</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" t="s">
         <v>74</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" t="s">
         <v>16</v>
       </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="E62" t="s">
+        <v>76</v>
+      </c>
+      <c r="F62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" t="s">
         <v>18</v>
       </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" t="s">
-        <v>17</v>
-      </c>
-      <c r="E37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" t="s">
-        <v>84</v>
-      </c>
-      <c r="E42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" t="s">
-        <v>85</v>
+      <c r="E63" t="s">
+        <v>76</v>
+      </c>
+      <c r="F63" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>